<commit_message>
add file read protected xlsx
</commit_message>
<xml_diff>
--- a/data/raw/input.xlsx
+++ b/data/raw/input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KNT21617\Downloads\newken\project\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA7AE709-1CDB-40BC-AEC6-BBE989CC3904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C3CEE76-6D80-451A-AF30-88E1C4BF8A36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -353,7 +353,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>